<commit_message>
Morphine Microglia Revision Work
</commit_message>
<xml_diff>
--- a/Morphine Microglia (unpublished)/Figure 2 Behavior/Behavior/NaloxoneBehavior.xlsx
+++ b/Morphine Microglia (unpublished)/Figure 2 Behavior/Behavior/NaloxoneBehavior.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Neumaier Lab\Morphine Grant\Behavioral Figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\GitHub\Manuscripts\Morphine Microglia (unpublished)\Figure 2 Behavior\Behavior\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="18">
   <si>
     <t>Treatment</t>
   </si>
@@ -60,6 +60,21 @@
   </si>
   <si>
     <t>SS</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -401,355 +416,476 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2">
         <v>3942.29</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>586.26099999999997</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>460.46199999999999</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
         <v>433.36399999999998</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>1145.19</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>1123.26</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
         <v>193.571</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>1068.5899999999999</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>1184.19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
         <v>1230.56</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>874.52499999999998</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>989.82299999999998</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
         <v>503.48200000000003</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>1090.06</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>1110.79</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
         <v>717.21500000000003</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>987.65700000000004</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>1120.96</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
         <v>8515.1</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>674.72699999999998</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>141.03200000000001</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9">
         <v>9268.9500000000007</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>486.96199999999999</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>118.532</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
         <v>12607.5</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>240.73099999999999</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>78.499200000000002</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
         <v>16579.599999999999</v>
       </c>
-      <c r="C11">
+      <c r="E11">
         <v>646.42700000000002</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>51.232799999999997</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12">
         <v>17571.5</v>
       </c>
-      <c r="C12">
+      <c r="E12">
         <v>476.262</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>21.4998</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13">
         <v>2039.12</v>
       </c>
-      <c r="C13">
+      <c r="E13">
         <v>738.55899999999997</v>
       </c>
-      <c r="D13">
+      <c r="F13">
         <v>767.19200000000001</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14">
         <v>3355.1</v>
       </c>
-      <c r="C14">
+      <c r="E14">
         <v>384.39600000000002</v>
       </c>
-      <c r="D14">
+      <c r="F14">
         <v>448.46199999999999</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15">
         <v>2792.15</v>
       </c>
-      <c r="C15">
+      <c r="E15">
         <v>478.79500000000002</v>
       </c>
-      <c r="D15">
+      <c r="F15">
         <v>593.86099999999999</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16">
         <v>3112.17</v>
       </c>
-      <c r="C16">
+      <c r="E16">
         <v>637.86</v>
       </c>
-      <c r="D16">
+      <c r="F16">
         <v>500.59500000000003</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17">
         <v>3389.26</v>
       </c>
-      <c r="C17">
+      <c r="E17">
         <v>617.62699999999995</v>
       </c>
-      <c r="D17">
+      <c r="F17">
         <v>584.39400000000001</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18">
         <v>4848.58</v>
       </c>
-      <c r="C18">
+      <c r="E18">
         <v>501.36200000000002</v>
       </c>
-      <c r="D18">
+      <c r="F18">
         <v>434.99599999999998</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19">
         <v>4467.1499999999996</v>
       </c>
-      <c r="C19">
+      <c r="E19">
         <v>472.19499999999999</v>
       </c>
-      <c r="D19">
+      <c r="F19">
         <v>424.029</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20">
         <v>4032.56</v>
       </c>
-      <c r="C20">
+      <c r="E20">
         <v>399.26299999999998</v>
       </c>
-      <c r="D20">
+      <c r="F20">
         <v>518.19500000000005</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>